<commit_message>
menampilkan product di halaman product
</commit_message>
<xml_diff>
--- a/database/FileExcel/Barang.xlsx
+++ b/database/FileExcel/Barang.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yovie\persediaanapp-magang\database\FileExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E8A4FA-AE86-4C84-AECD-E8FA6542E6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DB09E7-E950-4EDE-B47D-7B125092CEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{19905B0D-1A8A-4576-91B2-29E87108E41B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -53,12 +53,6 @@
     <t>XL</t>
   </si>
   <si>
-    <t>XXL</t>
-  </si>
-  <si>
-    <t>3XL</t>
-  </si>
-  <si>
     <t>created_at</t>
   </si>
   <si>
@@ -89,61 +83,79 @@
     <t>Anchor</t>
   </si>
   <si>
-    <t>Basic</t>
-  </si>
-  <si>
-    <t>Snow</t>
-  </si>
-  <si>
-    <t>Wolferine</t>
-  </si>
-  <si>
-    <t>Hopeless</t>
-  </si>
-  <si>
-    <t>No Love</t>
-  </si>
-  <si>
-    <t>Rose Coloured</t>
-  </si>
-  <si>
     <t>Daisy</t>
   </si>
   <si>
-    <t>Grass</t>
-  </si>
-  <si>
     <t>anchor</t>
   </si>
   <si>
-    <t>basic</t>
-  </si>
-  <si>
-    <t>snow</t>
-  </si>
-  <si>
-    <t>wolferine</t>
-  </si>
-  <si>
-    <t>hopeless</t>
-  </si>
-  <si>
-    <t>no-love</t>
-  </si>
-  <si>
-    <t>rose-coloured</t>
-  </si>
-  <si>
     <t>daisy</t>
   </si>
   <si>
-    <t>grass</t>
-  </si>
-  <si>
-    <t>Basic Red</t>
-  </si>
-  <si>
-    <t>basic-red</t>
+    <t>Mistake</t>
+  </si>
+  <si>
+    <t>mistake</t>
+  </si>
+  <si>
+    <t>Licate</t>
+  </si>
+  <si>
+    <t>licate</t>
+  </si>
+  <si>
+    <t>Crew</t>
+  </si>
+  <si>
+    <t>crew</t>
+  </si>
+  <si>
+    <t>Poppunk Suck</t>
+  </si>
+  <si>
+    <t>poppunk-suck</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>Basic Gn</t>
+  </si>
+  <si>
+    <t>basic-gn</t>
+  </si>
+  <si>
+    <t>Basic Logo</t>
+  </si>
+  <si>
+    <t>basic-logo</t>
+  </si>
+  <si>
+    <t>Basic Bk</t>
+  </si>
+  <si>
+    <t>basic-bk</t>
+  </si>
+  <si>
+    <t>Slop Anchor</t>
+  </si>
+  <si>
+    <t>slop-anchor</t>
+  </si>
+  <si>
+    <t>Sunglass Basic</t>
+  </si>
+  <si>
+    <t>sunglass-basic</t>
+  </si>
+  <si>
+    <t>Trapped</t>
+  </si>
+  <si>
+    <t>trapped</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -502,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D11C854-874A-442C-A5E8-60B8A1614FD1}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -527,34 +539,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
       <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -565,10 +577,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2">
         <v>65000</v>
@@ -577,13 +589,13 @@
         <v>130000</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -596,10 +608,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2">
         <v>65000</v>
@@ -608,13 +620,13 @@
         <v>130000</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
         <v>3</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -627,10 +639,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2">
         <v>65000</v>
@@ -639,13 +651,13 @@
         <v>130000</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -655,28 +667,28 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
-        <v>65000</v>
+        <v>90000</v>
       </c>
       <c r="F5" s="2">
-        <v>130000</v>
+        <v>185000</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -689,25 +701,25 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2">
-        <v>180000</v>
+        <v>90000</v>
       </c>
       <c r="F6" s="2">
-        <v>375000</v>
+        <v>185000</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
         <v>3</v>
       </c>
       <c r="I6">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -717,28 +729,28 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2">
-        <v>180000</v>
+        <v>75000</v>
       </c>
       <c r="F7" s="2">
-        <v>375000</v>
+        <v>145000</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -748,28 +760,28 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2">
-        <v>250000</v>
+        <v>50000</v>
       </c>
       <c r="F8" s="2">
-        <v>580000</v>
+        <v>110000</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -782,25 +794,25 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="F9" s="2">
-        <v>100000</v>
+        <v>110000</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -810,28 +822,28 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>60000</v>
+        <v>85000</v>
       </c>
       <c r="F10" s="2">
-        <v>110000</v>
+        <v>150000</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="I10">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -841,31 +853,118 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
-        <v>60000</v>
+        <v>95000</v>
       </c>
       <c r="F11" s="2">
-        <v>110000</v>
+        <v>185000</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="I11">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="2">
+        <v>75000</v>
+      </c>
+      <c r="F12" s="2">
+        <v>145000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2">
+        <v>90000</v>
+      </c>
+      <c r="F13" s="2">
+        <v>210000</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2">
+        <v>35000</v>
+      </c>
+      <c r="F14" s="2">
+        <v>80000</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>